<commit_message>
feat: 10 first movements no JSONs
</commit_message>
<xml_diff>
--- a/Requirements/Errores a detectar en acciones AECQ - fase 1.xlsx
+++ b/Requirements/Errores a detectar en acciones AECQ - fase 1.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{452D157C-D626-5143-92F6-A18F0310C1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UDLA\Capstone Project\Repo\Requirements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F9524C0-ACCA-41D8-82EE-71440A46FB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
   <si>
     <t>Errores a detectar en acciones - AECQ</t>
   </si>
@@ -377,7 +382,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -672,7 +677,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -692,7 +697,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -755,6 +760,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,57 +836,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -894,7 +899,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -946,7 +951,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1150,45 +1155,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5625" customWidth="1"/>
-    <col min="3" max="3" width="22.1953125" customWidth="1"/>
-    <col min="4" max="4" width="18.4296875" customWidth="1"/>
-    <col min="5" max="5" width="27.84375" customWidth="1"/>
-    <col min="6" max="6" width="17.484375" customWidth="1"/>
-    <col min="7" max="7" width="14.9296875" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1210,7 +1215,7 @@
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1236,28 +1241,28 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="28" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="45" t="s">
         <v>111</v>
       </c>
       <c r="J5" s="1"/>
@@ -1276,12 +1281,12 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+    <row r="6" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1291,7 +1296,7 @@
       <c r="H6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="29"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1308,14 +1313,14 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
     </row>
-    <row r="7" spans="1:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52" t="s">
+    <row r="7" spans="1:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="31" t="s">
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1352,10 +1357,10 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
     </row>
-    <row r="8" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
+    <row r="8" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1388,10 +1393,10 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
-    <row r="9" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
+    <row r="9" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1426,10 +1431,10 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
-    <row r="10" spans="1:24" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="38"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
+    <row r="10" spans="1:24" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
@@ -1464,10 +1469,10 @@
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
-    <row r="11" spans="1:24" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
+    <row r="11" spans="1:24" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="2" t="s">
         <v>61</v>
       </c>
@@ -1500,10 +1505,10 @@
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
-    <row r="12" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
+    <row r="12" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1536,10 +1541,10 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
     </row>
-    <row r="13" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
+    <row r="13" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1572,10 +1577,10 @@
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
     </row>
-    <row r="14" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="38"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
+    <row r="14" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="2" t="s">
         <v>63</v>
       </c>
@@ -1608,10 +1613,10 @@
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
     </row>
-    <row r="15" spans="1:24" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
+    <row r="15" spans="1:24" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="16" t="s">
         <v>103</v>
       </c>
@@ -1644,14 +1649,14 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
     </row>
-    <row r="16" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+    <row r="16" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="35" t="s">
         <v>65</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -1688,10 +1693,10 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
     </row>
-    <row r="17" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
+    <row r="17" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1724,10 +1729,10 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
     </row>
-    <row r="18" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
+    <row r="18" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="29"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1760,10 +1765,10 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
     </row>
-    <row r="19" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="38"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
+    <row r="19" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1798,10 +1803,10 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
     </row>
-    <row r="20" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+    <row r="20" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1834,10 +1839,10 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
     </row>
-    <row r="21" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
+    <row r="21" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1872,10 +1877,10 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
     </row>
-    <row r="22" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
+    <row r="22" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1908,10 +1913,10 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
-    <row r="23" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
+    <row r="23" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1944,10 +1949,10 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
     </row>
-    <row r="24" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="38"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
+    <row r="24" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1982,10 +1987,10 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
     </row>
-    <row r="25" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="38"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
+    <row r="25" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="29"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
@@ -2018,10 +2023,10 @@
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
     </row>
-    <row r="26" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="38"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
+    <row r="26" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="2" t="s">
         <v>69</v>
       </c>
@@ -2054,10 +2059,10 @@
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
     </row>
-    <row r="27" spans="1:24" ht="42" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
+    <row r="27" spans="1:24" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="30"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="16" t="s">
         <v>102</v>
       </c>
@@ -2090,14 +2095,14 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="1:24" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37" t="s">
+    <row r="28" spans="1:24" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="14" t="s">
@@ -2134,10 +2139,10 @@
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
     </row>
-    <row r="29" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="38"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
+    <row r="29" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -2170,10 +2175,10 @@
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
     </row>
-    <row r="30" spans="1:24" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="38"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
+    <row r="30" spans="1:24" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
       <c r="D30" s="2" t="s">
         <v>23</v>
       </c>
@@ -2206,10 +2211,10 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
     </row>
-    <row r="31" spans="1:24" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="38"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
+    <row r="31" spans="1:24" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
       <c r="D31" s="2" t="s">
         <v>24</v>
       </c>
@@ -2244,10 +2249,10 @@
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
     </row>
-    <row r="32" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="38"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
+    <row r="32" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="2" t="s">
         <v>75</v>
       </c>
@@ -2280,10 +2285,10 @@
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
     </row>
-    <row r="33" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="38"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
+    <row r="33" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="2" t="s">
         <v>29</v>
       </c>
@@ -2316,10 +2321,10 @@
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
     </row>
-    <row r="34" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="38"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
+    <row r="34" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="29"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="2" t="s">
         <v>77</v>
       </c>
@@ -2352,10 +2357,10 @@
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
     </row>
-    <row r="35" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="38"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
+    <row r="35" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="29"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
@@ -2390,10 +2395,10 @@
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
     </row>
-    <row r="36" spans="1:24" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="38"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
+    <row r="36" spans="1:24" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="2" t="s">
         <v>69</v>
       </c>
@@ -2426,10 +2431,10 @@
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
     </row>
-    <row r="37" spans="1:24" ht="28.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
+    <row r="37" spans="1:24" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="30"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="16" t="s">
         <v>108</v>
       </c>
@@ -2464,14 +2469,14 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="1:24" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="49" t="s">
+    <row r="38" spans="1:24" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="42" t="s">
         <v>81</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -2508,10 +2513,10 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="50"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
+    <row r="39" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
       <c r="D39" s="2" t="s">
         <v>82</v>
       </c>
@@ -2546,10 +2551,10 @@
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
     </row>
-    <row r="40" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
+    <row r="40" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
       <c r="D40" s="2" t="s">
         <v>83</v>
       </c>
@@ -2584,10 +2589,10 @@
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
     </row>
-    <row r="41" spans="1:24" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="50"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
+    <row r="41" spans="1:24" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
       <c r="D41" s="2" t="s">
         <v>85</v>
       </c>
@@ -2620,10 +2625,10 @@
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
     </row>
-    <row r="42" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="50"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
+    <row r="42" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
       <c r="D42" s="4" t="s">
         <v>42</v>
       </c>
@@ -2656,10 +2661,10 @@
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
     </row>
-    <row r="43" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="50"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
+    <row r="43" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
       <c r="D43" s="4" t="s">
         <v>43</v>
       </c>
@@ -2694,10 +2699,10 @@
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
     </row>
-    <row r="44" spans="1:24" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="51"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
+    <row r="44" spans="1:24" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
       <c r="D44" s="7" t="s">
         <v>44</v>
       </c>
@@ -2730,14 +2735,14 @@
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
     </row>
-    <row r="45" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="43" t="s">
+    <row r="45" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="35" t="s">
         <v>89</v>
       </c>
       <c r="D45" s="19" t="s">
@@ -2774,10 +2779,10 @@
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
     </row>
-    <row r="46" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="44"/>
-      <c r="B46" s="47"/>
-      <c r="C46" s="41"/>
+    <row r="46" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="37"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="32"/>
       <c r="D46" s="4" t="s">
         <v>50</v>
       </c>
@@ -2812,10 +2817,10 @@
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
     </row>
-    <row r="47" spans="1:24" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="44"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="41"/>
+    <row r="47" spans="1:24" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="37"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="32"/>
       <c r="D47" s="4" t="s">
         <v>51</v>
       </c>
@@ -2831,7 +2836,9 @@
       <c r="H47" s="21">
         <v>0.3</v>
       </c>
-      <c r="I47" s="27"/>
+      <c r="I47" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -2848,10 +2855,10 @@
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
     </row>
-    <row r="48" spans="1:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="44"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="41"/>
+    <row r="48" spans="1:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="37"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="32"/>
       <c r="D48" s="4" t="s">
         <v>52</v>
       </c>
@@ -2886,10 +2893,10 @@
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
     </row>
-    <row r="49" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="44"/>
-      <c r="B49" s="47"/>
-      <c r="C49" s="41"/>
+    <row r="49" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="37"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="32"/>
       <c r="D49" s="4" t="s">
         <v>91</v>
       </c>
@@ -2922,10 +2929,10 @@
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
     </row>
-    <row r="50" spans="1:24" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="44"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="41"/>
+    <row r="50" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="37"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="4" t="s">
         <v>92</v>
       </c>
@@ -2958,10 +2965,10 @@
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
     </row>
-    <row r="51" spans="1:24" ht="54.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="44"/>
-      <c r="B51" s="47"/>
-      <c r="C51" s="41"/>
+    <row r="51" spans="1:24" ht="63" x14ac:dyDescent="0.25">
+      <c r="A51" s="37"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="4" t="s">
         <v>94</v>
       </c>
@@ -2996,10 +3003,10 @@
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
     </row>
-    <row r="52" spans="1:24" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A52" s="44"/>
-      <c r="B52" s="47"/>
-      <c r="C52" s="41"/>
+    <row r="52" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="37"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="32"/>
       <c r="D52" s="4" t="s">
         <v>95</v>
       </c>
@@ -3032,10 +3039,10 @@
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
     </row>
-    <row r="53" spans="1:24" ht="54.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="44"/>
-      <c r="B53" s="47"/>
-      <c r="C53" s="41"/>
+    <row r="53" spans="1:24" ht="63" x14ac:dyDescent="0.25">
+      <c r="A53" s="37"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="32"/>
       <c r="D53" s="4" t="s">
         <v>96</v>
       </c>
@@ -3068,10 +3075,10 @@
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
     </row>
-    <row r="54" spans="1:24" ht="55.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="42"/>
+    <row r="54" spans="1:24" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="38"/>
+      <c r="B54" s="41"/>
+      <c r="C54" s="33"/>
       <c r="D54" s="16" t="s">
         <v>105</v>
       </c>
@@ -3104,7 +3111,7 @@
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3132,21 +3139,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A7:A15"/>
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="C7:C15"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="B16:B27"/>
-    <mergeCell ref="C16:C27"/>
-    <mergeCell ref="A28:A37"/>
-    <mergeCell ref="B28:B37"/>
-    <mergeCell ref="C28:C37"/>
-    <mergeCell ref="A45:A54"/>
-    <mergeCell ref="B45:B54"/>
-    <mergeCell ref="C45:C54"/>
-    <mergeCell ref="A38:A44"/>
-    <mergeCell ref="B38:B44"/>
-    <mergeCell ref="C38:C44"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
@@ -3157,6 +3149,21 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A28:A37"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="C28:C37"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="B45:B54"/>
+    <mergeCell ref="C45:C54"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="C38:C44"/>
+    <mergeCell ref="A7:A15"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="B16:B27"/>
+    <mergeCell ref="C16:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3164,20 +3171,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8b5aa52d-55c6-460f-b140-7d1036289c34" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8b5aa52d-55c6-460f-b140-7d1036289c34" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3416,20 +3423,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D7CCF83-8457-4566-ABFC-3A668131BC08}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D691B179-DAC8-4892-8EEB-E7FC955684C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
-    <ds:schemaRef ds:uri="8b5aa52d-55c6-460f-b140-7d1036289c34"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D691B179-DAC8-4892-8EEB-E7FC955684C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D7CCF83-8457-4566-ABFC-3A668131BC08}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="8b5aa52d-55c6-460f-b140-7d1036289c34"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a7a475fa-823d-4b6d-a5c9-7ed2d4452183"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3443,6 +3456,13 @@
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="8b5aa52d-55c6-460f-b140-7d1036289c34"/>
     <ds:schemaRef ds:uri="a7a475fa-823d-4b6d-a5c9-7ed2d4452183"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>